<commit_message>
My commit to QA
</commit_message>
<xml_diff>
--- a/excel_file.xlsx
+++ b/excel_file.xlsx
@@ -348,7 +348,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,7 +374,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -382,7 +382,7 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -398,7 +398,7 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>